<commit_message>
Updated sheet with expected coins-per day
</commit_message>
<xml_diff>
--- a/Verus_POS.xlsx
+++ b/Verus_POS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Klanten\Brink, F. van den\Financiëel\Crypto\VRSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E374204-D421-4AA7-B9EC-FE0DE8C764FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7266F9C-9CC1-4E5A-888F-0406B0CBC35D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="25200" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verus POS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>This spreadsheet was made for fast and easy access to key numbers</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Spreadsheet made by @Cragorn &amp; edited by @Oink on Verus Discord.</t>
+  </si>
+  <si>
+    <t>Expected average VRSC/day adjusted for % staking</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
     <numFmt numFmtId="164" formatCode="0.0000\ %"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -207,6 +210,13 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -229,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -417,11 +427,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -432,12 +457,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,22 +481,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,7 +502,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -871,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:P1015"/>
+  <dimension ref="B5:P1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -899,22 +931,22 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -922,824 +954,830 @@
       <c r="D9" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="40">
+      <c r="B11" s="33">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5">
-        <v>660436</v>
-      </c>
-      <c r="G11" s="29" t="s">
+        <v>678594</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="29" t="s">
+        <v>87659</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="40">
+      <c r="B15" s="41">
         <v>2</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="11">
-        <f>SUM(D23:D35)+D39</f>
-        <v>30732056.120000001</v>
-      </c>
-      <c r="G15" s="29" t="s">
+      <c r="D15" s="43">
+        <f>SUM(D24:D36)+D40</f>
+        <v>31597647.98</v>
+      </c>
+      <c r="G15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="46">
         <f>D12/D15</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="29" t="s">
+        <v>2.7742254757532748E-3</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="47">
         <f>D16*720</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="29" t="s">
+        <v>1.997442342542358</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="43">
         <f>D15*D13</f>
-        <v>30732056.120000001</v>
-      </c>
-      <c r="G18" s="29" t="s">
+        <v>31597647.98</v>
+      </c>
+      <c r="G18" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="47">
         <f>D12/D18*720</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="33">
+        <v>1.997442342542358</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="48"/>
+      <c r="C20" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="47">
+        <f>D19*IF(F57&gt;0,IF(F56,IF(F55&gt;0,IF(F54&gt;0,IF(F53&gt;0,IF(F52&gt;0,IF(F51&gt;0,IF(F50,IF(F49&gt;0,IF(F48&gt;0,IF(F47&gt;0,IF(F46&gt;0,IF(F45&gt;0,C44,C45),C46),C47),C48),C49),C50),C51),C52),C53),C54),C55),C56),C57)</f>
+        <v>47.938616221016588</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="39">
         <v>3</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C22" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
-      <c r="C22" s="16" t="s">
+      <c r="D22" s="36"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E23" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
-      <c r="C23" s="19" t="s">
+    <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D24" s="15">
         <v>485000</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E24" s="16">
         <v>485000</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="19" t="s">
+    <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="20">
-        <f>IF($D$11&gt;E44, IF($D$11&gt;E45, C45*(E45-E44), ($D$11-E44)*C45), 0)</f>
+      <c r="D25" s="15">
+        <f t="shared" ref="D25:D36" si="0">IF($D$11&gt;E45, IF($D$11&gt;E46, C46*(E46-E45), ($D$11-E45)*C46), 0)</f>
         <v>4147200</v>
       </c>
-      <c r="E24" s="21">
-        <f>C45*(E45-E44)</f>
+      <c r="E25" s="16">
+        <f t="shared" ref="E25:E36" si="1">C46*(E46-E45)</f>
         <v>4147200</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
-      <c r="C25" s="19" t="s">
+    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="20">
-        <f>IF($D$11&gt;E45, IF($D$11&gt;E46, C46*(E46-E45), ($D$11-E45)*C46), 0)</f>
+      <c r="D26" s="15">
+        <f t="shared" si="0"/>
         <v>2073600</v>
       </c>
-      <c r="E25" s="21">
-        <f>C46*(E46-E45)</f>
+      <c r="E26" s="16">
+        <f t="shared" si="1"/>
         <v>2073600</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="34"/>
-      <c r="C26" s="19" t="s">
+    <row r="27" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="20">
-        <f>IF($D$11&gt;E46, IF($D$11&gt;E47, C47*(E47-E46), ($D$11-E46)*C47), 0)</f>
-        <v>11461368</v>
-      </c>
-      <c r="E26" s="21">
-        <f>C47*(E47-E46)</f>
+      <c r="D27" s="15">
+        <f t="shared" si="0"/>
+        <v>11897160</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" si="1"/>
         <v>26282880</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="34"/>
-      <c r="C27" s="19" t="s">
+    <row r="28" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="20">
-        <f>IF($D$11&gt;E47, IF($D$11&gt;E48, C48*(E48-E47), ($D$11-E47)*C48), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="21">
-        <f>C48*(E48-E47)</f>
-        <v>12623040</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="20">
-        <f>IF($D$11&gt;E48, IF($D$11&gt;E49, C49*(E49-E48), ($D$11-E48)*C49), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="21">
-        <f>C49*(E49-E48)</f>
-        <v>6311520</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="34"/>
-      <c r="C29" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="20">
-        <f>IF($D$11&gt;E49, IF($D$11&gt;E50, C50*(E50-E49), ($D$11-E49)*C50), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="21">
-        <f>C50*(E50-E49)</f>
-        <v>3155760</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="34"/>
-      <c r="C30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="20">
-        <f>IF($D$11&gt;E50, IF($D$11&gt;E51, C51*(E51-E50), ($D$11-E50)*C51), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="21">
-        <f>C51*(E51-E50)</f>
-        <v>1577880</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="34"/>
-      <c r="C31" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="20">
-        <f>IF($D$11&gt;E51, IF($D$11&gt;E52, C52*(E52-E51), ($D$11-E51)*C52), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="21">
-        <f>C52*(E52-E51)</f>
-        <v>788940</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
-      <c r="C32" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="20">
-        <f>IF($D$11&gt;E52, IF($D$11&gt;E53, C53*(E53-E52), ($D$11-E52)*C53), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="21">
-        <f>C53*(E53-E52)</f>
-        <v>394470</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="34"/>
-      <c r="C33" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="20">
-        <f>IF($D$11&gt;E53, IF($D$11&gt;E54, C54*(E54-E53), ($D$11-E53)*C54), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="21">
-        <f>C54*(E54-E53)</f>
-        <v>197235</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="34"/>
-      <c r="C34" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="20">
-        <f>IF($D$11&gt;E54, IF($D$11&gt;E55, C55*(E55-E54), ($D$11-E54)*C55), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="21">
-        <f>C55*(E55-E54)</f>
-        <v>98617.5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
-      <c r="C35" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="20">
-        <f>IF($D$11&gt;E55, IF($D$11&gt;E56, C56*(E56-E55), ($D$11-E55)*C56), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="21">
-        <f>C56*(E56-E55)</f>
-        <v>49308.75</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35">
-        <v>4</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="39"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="24">
-        <v>23.67</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="37"/>
-      <c r="C39" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="23">
-        <f>IF($D$11&lt;129600, 0, IF($D$11&gt;1181520, (1181520-129600)*D38, ($D$11-129600)*D38))</f>
-        <v>12564888.120000001</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="31">
-        <v>5</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="32"/>
-      <c r="C42" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="14">
-        <v>0</v>
-      </c>
-      <c r="E42" s="14">
-        <v>10079</v>
-      </c>
-      <c r="F42" s="28">
-        <f t="shared" ref="F42:F56" si="0">IF($D$11&gt;D42, 0, (D42-$D$11)/1440)</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="28">
-        <f>F42/365.2425</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="32"/>
-      <c r="C43" s="27">
-        <v>384</v>
-      </c>
-      <c r="D43" s="14">
-        <v>10080</v>
-      </c>
-      <c r="E43" s="14">
-        <f t="shared" ref="E43:E46" si="1">D43+43200-1</f>
-        <v>53279</v>
-      </c>
-      <c r="F43" s="28">
+      <c r="D28" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G43" s="28">
-        <f t="shared" ref="G43:G56" si="2">F43/365.2425</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="32"/>
-      <c r="C44" s="27">
-        <f>C43/2</f>
-        <v>192</v>
-      </c>
-      <c r="D44" s="14">
-        <f t="shared" ref="D44:D48" si="3">E43+1</f>
-        <v>53280</v>
-      </c>
-      <c r="E44" s="14">
+      <c r="E28" s="16">
         <f t="shared" si="1"/>
-        <v>96479</v>
-      </c>
-      <c r="F44" s="28">
+        <v>12623040</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G44" s="28">
+      <c r="E29" s="16">
+        <f t="shared" si="1"/>
+        <v>6311520</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="16">
+        <f t="shared" si="1"/>
+        <v>3155760</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="16">
+        <f t="shared" si="1"/>
+        <v>1577880</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <f t="shared" si="1"/>
+        <v>788940</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="40"/>
+      <c r="C33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <f t="shared" si="1"/>
+        <v>394470</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="40"/>
+      <c r="C34" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <f t="shared" si="1"/>
+        <v>197235</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="40"/>
+      <c r="C35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <f t="shared" si="1"/>
+        <v>98617.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="40"/>
+      <c r="C36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <f t="shared" si="1"/>
+        <v>49308.75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="28">
+        <v>4</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="32"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="29"/>
+      <c r="C39" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="19">
+        <v>23.67</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="30"/>
+      <c r="C40" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="18">
+        <f>IF($D$11&lt;129600, 0, IF($D$11&gt;1181520, (1181520-129600)*D39, ($D$11-129600)*D39))</f>
+        <v>12994687.98</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="37">
+        <v>5</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="38"/>
+      <c r="C43" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
+        <v>10079</v>
+      </c>
+      <c r="F43" s="23">
+        <f t="shared" ref="F43:F57" si="2">IF($D$11&gt;D43, 0, (D43-$D$11)/1440)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="23">
+        <f>F43/365.2425</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="38"/>
+      <c r="C44" s="22">
+        <v>384</v>
+      </c>
+      <c r="D44" s="10">
+        <v>10080</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" ref="E44:E47" si="3">D44+43200-1</f>
+        <v>53279</v>
+      </c>
+      <c r="F44" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G44" s="23">
+        <f t="shared" ref="G44:G57" si="4">F44/365.2425</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="32"/>
-      <c r="C45" s="27">
-        <f t="shared" ref="C45:C56" si="4">C44/2</f>
-        <v>96</v>
-      </c>
-      <c r="D45" s="14">
+      <c r="B45" s="38"/>
+      <c r="C45" s="22">
+        <f>C44/2</f>
+        <v>192</v>
+      </c>
+      <c r="D45" s="10">
+        <f t="shared" ref="D45:D49" si="5">E44+1</f>
+        <v>53280</v>
+      </c>
+      <c r="E45" s="10">
         <f t="shared" si="3"/>
-        <v>96480</v>
-      </c>
-      <c r="E45" s="14">
-        <f t="shared" si="1"/>
-        <v>139679</v>
-      </c>
-      <c r="F45" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="28">
+        <v>96479</v>
+      </c>
+      <c r="F45" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G45" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="32"/>
-      <c r="C46" s="27">
-        <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-      <c r="D46" s="14">
+      <c r="B46" s="38"/>
+      <c r="C46" s="22">
+        <f t="shared" ref="C46:C57" si="6">C45/2</f>
+        <v>96</v>
+      </c>
+      <c r="D46" s="10">
+        <f t="shared" si="5"/>
+        <v>96480</v>
+      </c>
+      <c r="E46" s="10">
         <f t="shared" si="3"/>
-        <v>139680</v>
-      </c>
-      <c r="E46" s="14">
-        <f t="shared" si="1"/>
-        <v>182879</v>
-      </c>
-      <c r="F46" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="28">
+        <v>139679</v>
+      </c>
+      <c r="F46" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G46" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="32"/>
-      <c r="C47" s="27">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="D47" s="14">
+      <c r="B47" s="38"/>
+      <c r="C47" s="22">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="D47" s="10">
+        <f t="shared" si="5"/>
+        <v>139680</v>
+      </c>
+      <c r="E47" s="10">
         <f t="shared" si="3"/>
-        <v>182880</v>
-      </c>
-      <c r="E47" s="14">
-        <f>D47+43200+1051920-1</f>
-        <v>1277999</v>
-      </c>
-      <c r="F47" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="28">
+        <v>182879</v>
+      </c>
+      <c r="F47" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I47" s="44"/>
+      <c r="G47" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="32"/>
-      <c r="C48" s="27">
+      <c r="B48" s="38"/>
+      <c r="C48" s="22">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="D48" s="10">
+        <f t="shared" si="5"/>
+        <v>182880</v>
+      </c>
+      <c r="E48" s="10">
+        <f>D48+43200+1051920-1</f>
+        <v>1277999</v>
+      </c>
+      <c r="F48" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="23">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="24"/>
+    </row>
+    <row r="49" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="38"/>
+      <c r="C49" s="22">
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="D48" s="14">
-        <f t="shared" si="3"/>
+      <c r="D49" s="10">
+        <f t="shared" si="5"/>
         <v>1278000</v>
       </c>
-      <c r="E48" s="14">
-        <f>D48+1051920-1</f>
+      <c r="E49" s="10">
+        <f>D49+1051920-1</f>
         <v>2329919</v>
       </c>
-      <c r="F48" s="28">
-        <f t="shared" si="0"/>
-        <v>428.86388888888888</v>
-      </c>
-      <c r="G48" s="28">
+      <c r="F49" s="23">
         <f t="shared" si="2"/>
-        <v>1.1741894464332296</v>
-      </c>
-      <c r="I48" s="44"/>
-    </row>
-    <row r="49" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="32"/>
-      <c r="C49" s="27">
+        <v>416.25416666666666</v>
+      </c>
+      <c r="G49" s="23">
         <f t="shared" si="4"/>
+        <v>1.1396651996048288</v>
+      </c>
+      <c r="I49" s="24"/>
+    </row>
+    <row r="50" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="38"/>
+      <c r="C50" s="22">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="D49" s="14">
-        <f>E48+1</f>
+      <c r="D50" s="10">
+        <f>E49+1</f>
         <v>2329920</v>
       </c>
-      <c r="E49" s="14">
-        <f t="shared" ref="E49:E56" si="5">D49+1051920-1</f>
+      <c r="E50" s="10">
+        <f t="shared" ref="E50:E57" si="7">D50+1051920-1</f>
         <v>3381839</v>
       </c>
-      <c r="F49" s="28">
-        <f t="shared" si="0"/>
-        <v>1159.3638888888888</v>
-      </c>
-      <c r="G49" s="28">
+      <c r="F50" s="23">
         <f t="shared" si="2"/>
-        <v>3.1742305150383343</v>
-      </c>
-      <c r="I49" s="44"/>
-    </row>
-    <row r="50" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="32"/>
-      <c r="C50" s="27">
+        <v>1146.7541666666666</v>
+      </c>
+      <c r="G50" s="23">
         <f t="shared" si="4"/>
+        <v>3.1397062682099333</v>
+      </c>
+      <c r="I50" s="24"/>
+    </row>
+    <row r="51" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="38"/>
+      <c r="C51" s="22">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="D50" s="14">
-        <f t="shared" ref="D50:D56" si="6">E49+1</f>
+      <c r="D51" s="10">
+        <f t="shared" ref="D51:D57" si="8">E50+1</f>
         <v>3381840</v>
       </c>
-      <c r="E50" s="14">
-        <f t="shared" si="5"/>
+      <c r="E51" s="10">
+        <f t="shared" si="7"/>
         <v>4433759</v>
       </c>
-      <c r="F50" s="28">
-        <f t="shared" si="0"/>
-        <v>1889.8638888888888</v>
-      </c>
-      <c r="G50" s="28">
+      <c r="F51" s="23">
         <f t="shared" si="2"/>
-        <v>5.1742715836434394</v>
-      </c>
-      <c r="I50" s="44"/>
-    </row>
-    <row r="51" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="32"/>
-      <c r="C51" s="27">
+        <v>1877.2541666666666</v>
+      </c>
+      <c r="G51" s="23">
         <f t="shared" si="4"/>
+        <v>5.1397473368150379</v>
+      </c>
+      <c r="I51" s="24"/>
+    </row>
+    <row r="52" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="38"/>
+      <c r="C52" s="22">
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D52" s="10">
+        <f t="shared" si="8"/>
+        <v>4433760</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="7"/>
+        <v>5485679</v>
+      </c>
+      <c r="F52" s="23">
+        <f t="shared" si="2"/>
+        <v>2607.7541666666666</v>
+      </c>
+      <c r="G52" s="23">
+        <f t="shared" si="4"/>
+        <v>7.139788405420143</v>
+      </c>
+      <c r="I52" s="24"/>
+    </row>
+    <row r="53" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="38"/>
+      <c r="C53" s="22">
         <f t="shared" si="6"/>
-        <v>4433760</v>
-      </c>
-      <c r="E51" s="14">
-        <f t="shared" si="5"/>
-        <v>5485679</v>
-      </c>
-      <c r="F51" s="28">
-        <f t="shared" si="0"/>
-        <v>2620.3638888888891</v>
-      </c>
-      <c r="G51" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="D53" s="10">
+        <f t="shared" si="8"/>
+        <v>5485680</v>
+      </c>
+      <c r="E53" s="10">
+        <f t="shared" si="7"/>
+        <v>6537599</v>
+      </c>
+      <c r="F53" s="23">
         <f t="shared" si="2"/>
-        <v>7.1743126522485445</v>
-      </c>
-      <c r="I51" s="44"/>
-    </row>
-    <row r="52" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="32"/>
-      <c r="C52" s="27">
+        <v>3338.2541666666666</v>
+      </c>
+      <c r="G53" s="23">
         <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="D52" s="14">
+        <v>9.1398294740252481</v>
+      </c>
+      <c r="I53" s="24"/>
+    </row>
+    <row r="54" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="38"/>
+      <c r="C54" s="22">
         <f t="shared" si="6"/>
-        <v>5485680</v>
-      </c>
-      <c r="E52" s="14">
-        <f t="shared" si="5"/>
-        <v>6537599</v>
-      </c>
-      <c r="F52" s="28">
-        <f t="shared" si="0"/>
-        <v>3350.8638888888891</v>
-      </c>
-      <c r="G52" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="D54" s="10">
+        <f t="shared" si="8"/>
+        <v>6537600</v>
+      </c>
+      <c r="E54" s="10">
+        <f t="shared" si="7"/>
+        <v>7589519</v>
+      </c>
+      <c r="F54" s="23">
         <f t="shared" si="2"/>
-        <v>9.1743537208536488</v>
-      </c>
-      <c r="I52" s="44"/>
-    </row>
-    <row r="53" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="32"/>
-      <c r="C53" s="27">
+        <v>4068.7541666666666</v>
+      </c>
+      <c r="G54" s="23">
         <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="D53" s="14">
+        <v>11.139870542630353</v>
+      </c>
+      <c r="I54" s="24"/>
+    </row>
+    <row r="55" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="38"/>
+      <c r="C55" s="22">
         <f t="shared" si="6"/>
-        <v>6537600</v>
-      </c>
-      <c r="E53" s="14">
-        <f t="shared" si="5"/>
-        <v>7589519</v>
-      </c>
-      <c r="F53" s="28">
-        <f t="shared" si="0"/>
-        <v>4081.3638888888891</v>
-      </c>
-      <c r="G53" s="28">
+        <v>0.1875</v>
+      </c>
+      <c r="D55" s="10">
+        <f t="shared" si="8"/>
+        <v>7589520</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" si="7"/>
+        <v>8641439</v>
+      </c>
+      <c r="F55" s="23">
         <f t="shared" si="2"/>
-        <v>11.174394789458754</v>
-      </c>
-      <c r="I53" s="44"/>
-    </row>
-    <row r="54" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="32"/>
-      <c r="C54" s="27">
+        <v>4799.2541666666666</v>
+      </c>
+      <c r="G55" s="23">
         <f t="shared" si="4"/>
-        <v>0.1875</v>
-      </c>
-      <c r="D54" s="14">
+        <v>13.139911611235457</v>
+      </c>
+      <c r="I55" s="24"/>
+    </row>
+    <row r="56" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="38"/>
+      <c r="C56" s="22">
         <f t="shared" si="6"/>
-        <v>7589520</v>
-      </c>
-      <c r="E54" s="14">
-        <f t="shared" si="5"/>
-        <v>8641439</v>
-      </c>
-      <c r="F54" s="28">
-        <f t="shared" si="0"/>
-        <v>4811.8638888888891</v>
-      </c>
-      <c r="G54" s="28">
+        <v>9.375E-2</v>
+      </c>
+      <c r="D56" s="10">
+        <f t="shared" si="8"/>
+        <v>8641440</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="7"/>
+        <v>9693359</v>
+      </c>
+      <c r="F56" s="23">
         <f t="shared" si="2"/>
-        <v>13.174435858063859</v>
-      </c>
-      <c r="I54" s="44"/>
-    </row>
-    <row r="55" spans="2:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="32"/>
-      <c r="C55" s="27">
+        <v>5529.7541666666666</v>
+      </c>
+      <c r="G56" s="23">
         <f t="shared" si="4"/>
-        <v>9.375E-2</v>
-      </c>
-      <c r="D55" s="14">
+        <v>15.139952679840562</v>
+      </c>
+      <c r="I56" s="24"/>
+    </row>
+    <row r="57" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="38"/>
+      <c r="C57" s="22">
         <f t="shared" si="6"/>
-        <v>8641440</v>
-      </c>
-      <c r="E55" s="14">
-        <f t="shared" si="5"/>
-        <v>9693359</v>
-      </c>
-      <c r="F55" s="28">
-        <f t="shared" si="0"/>
-        <v>5542.3638888888891</v>
-      </c>
-      <c r="G55" s="28">
+        <v>4.6875E-2</v>
+      </c>
+      <c r="D57" s="10">
+        <f t="shared" si="8"/>
+        <v>9693360</v>
+      </c>
+      <c r="E57" s="10">
+        <f t="shared" si="7"/>
+        <v>10745279</v>
+      </c>
+      <c r="F57" s="23">
         <f t="shared" si="2"/>
-        <v>15.174476926668964</v>
-      </c>
-      <c r="I55" s="44"/>
-    </row>
-    <row r="56" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="32"/>
-      <c r="C56" s="27">
+        <v>6260.2541666666666</v>
+      </c>
+      <c r="G57" s="23">
         <f t="shared" si="4"/>
-        <v>4.6875E-2</v>
-      </c>
-      <c r="D56" s="14">
-        <f t="shared" si="6"/>
-        <v>9693360</v>
-      </c>
-      <c r="E56" s="14">
-        <f t="shared" si="5"/>
-        <v>10745279</v>
-      </c>
-      <c r="F56" s="28">
-        <f t="shared" si="0"/>
-        <v>6272.8638888888891</v>
-      </c>
-      <c r="G56" s="28">
-        <f t="shared" si="2"/>
-        <v>17.174517995274069</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>17.139993748445669</v>
+      </c>
+    </row>
     <row r="58" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="29" t="s">
+    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-    </row>
-    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="29" t="s">
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+    </row>
+    <row r="61" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61">
-        <v>10680479</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="29" t="s">
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+    </row>
+    <row r="63" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-    </row>
-    <row r="63" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="29" t="s">
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+    </row>
+    <row r="64" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-    </row>
-    <row r="64" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+    </row>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2691,19 +2729,13 @@
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B60:F60"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="G12:P12"/>
     <mergeCell ref="G13:P13"/>
@@ -2712,8 +2744,15 @@
     <mergeCell ref="G16:P16"/>
     <mergeCell ref="G17:P17"/>
     <mergeCell ref="G18:P18"/>
-    <mergeCell ref="B41:B56"/>
-    <mergeCell ref="B21:B35"/>
+    <mergeCell ref="B42:B57"/>
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>